<commit_message>
Commit - PDF, Word, Excel file handling
</commit_message>
<xml_diff>
--- a/tests/testFile1.xlsx
+++ b/tests/testFile1.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">celda a1</t>
   </si>
@@ -95,6 +96,81 @@
   </si>
   <si>
     <t xml:space="preserve">celda e5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new b1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new c1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new d1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new a2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new b2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new d2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new e2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new a3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new b3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new c3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new a4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new b4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new c4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new e4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new a5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new b5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new c5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new d5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new e5</t>
   </si>
 </sst>
 </file>
@@ -168,8 +244,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,94 +378,94 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -398,4 +478,113 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>